<commit_message>
Re-commit because of issues
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sprint 2 (M2)" sheetId="1" r:id="rId2"/>
+    <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,12 +20,104 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Set Up Git on team's machines</t>
+  </si>
+  <si>
+    <t>Edit and commit Person 1 class</t>
+  </si>
+  <si>
+    <t>Edit and commit Person 2 class</t>
+  </si>
+  <si>
+    <t>Edit and commit Person 3 class</t>
+  </si>
+  <si>
+    <t>Edit and commit Person 4 class</t>
+  </si>
+  <si>
+    <t>Edit and commit Person 5 class</t>
+  </si>
+  <si>
+    <t>Bhavesh</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Pranil</t>
+  </si>
+  <si>
+    <t>Naman</t>
+  </si>
+  <si>
+    <t>Create Build File 1</t>
+  </si>
+  <si>
+    <t>Create Build File 2</t>
+  </si>
+  <si>
+    <t>Create Build File 3</t>
+  </si>
+  <si>
+    <t>Create Build File 4</t>
+  </si>
+  <si>
+    <t>Create Build File 5</t>
+  </si>
+  <si>
+    <t>Not required</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +140,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,9 +503,239 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>

<commit_message>
Completed M3 of sprint_backlog.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\2014-2015\Fall 2014\CS 2340 Objects and Design\SpaceTraders2340\admin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>Tasks</t>
   </si>
@@ -84,6 +89,30 @@
   </si>
   <si>
     <t>Not required</t>
+  </si>
+  <si>
+    <t>Create Context Diagram</t>
+  </si>
+  <si>
+    <t>Collate the best use cases</t>
+  </si>
+  <si>
+    <t>Brainstorm 10 use cases</t>
+  </si>
+  <si>
+    <t>Handle player object creation and game configuration dialog mechanics (5 &amp; 6)</t>
+  </si>
+  <si>
+    <t>Create Space Trader FX project (1)</t>
+  </si>
+  <si>
+    <t>Design Welcome Screen UI (2)</t>
+  </si>
+  <si>
+    <t>Implement pressing "New Game" to access the game configuration dialog (3)</t>
+  </si>
+  <si>
+    <t>Implement character creation (name + skill points) (4)</t>
   </si>
 </sst>
 </file>
@@ -176,6 +205,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -507,12 +544,12 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -531,19 +568,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -580,7 +617,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -594,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -608,7 +645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -622,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -636,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -650,7 +687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -664,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -678,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -692,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -706,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -733,12 +770,209 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Finished Sprint 4. Fixed commit message with force.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\2014-2015\Fall 2014\CS 2340 Objects and Design\SpaceTraders2340\admin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18260" windowHeight="16240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
     <sheet name="Sprint 2 (M2)" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
   <si>
     <t>Tasks</t>
   </si>
@@ -113,13 +109,34 @@
   </si>
   <si>
     <t>Implement character creation (name + skill points) (4)</t>
+  </si>
+  <si>
+    <t>Develop and map out architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hunter </t>
+  </si>
+  <si>
+    <t>Create framework of classes from architecture</t>
+  </si>
+  <si>
+    <t>Create generators</t>
+  </si>
+  <si>
+    <t>Create dump abilities</t>
+  </si>
+  <si>
+    <t>Cleanup, readover, code critique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Started </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +168,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -169,7 +193,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -179,8 +203,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,16 +225,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,12 +591,12 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -572,15 +619,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="2"/>
+    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="31.5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -617,7 +664,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="31.5">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -631,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -645,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -659,7 +706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="31.5">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -673,7 +720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="31.5">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -687,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -701,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -715,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -729,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -743,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -770,18 +817,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.25" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -818,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -832,7 +879,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -846,7 +893,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -860,7 +907,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -874,7 +921,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -888,7 +935,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -902,7 +949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -916,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -930,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="47.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -944,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -958,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="47.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -972,8 +1019,142 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Edited Sprint Backlog. Updated completion times and added totals.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18260" windowHeight="16240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
   <si>
     <t>Tasks</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve">Not Started </t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,6 +231,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -613,10 +617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -664,7 +668,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -678,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -692,7 +696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -706,7 +710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -720,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -802,6 +806,15 @@
       </c>
       <c r="D12" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1">
+        <f>SUM(D2:D12)</f>
+        <v>15.5</v>
       </c>
     </row>
   </sheetData>
@@ -817,10 +830,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -828,7 +841,7 @@
     <col min="1" max="1" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,10 +987,10 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="47.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -988,10 +1001,10 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1002,10 +1015,10 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="47.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1016,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1031,6 +1044,15 @@
       </c>
       <c r="D14" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5">
+        <f>SUM(D2:D14)</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1046,11 +1068,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1107,7 +1127,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1135,7 +1155,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30">
@@ -1150,6 +1170,15 @@
       </c>
       <c r="D6" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1">
+        <f>SUM(D2:D6)</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added features to Person 1
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Tasks</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -619,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -662,10 +665,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>0.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
@@ -832,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated sprint_backlog to edit status of task #6
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -724,7 +724,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
I was person 5. I added my readme text file, deleted my useless text file, wrote a method in my Person java file, and updated the sprint backlog
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -141,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -591,16 +591,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -619,19 +619,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -657,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="31.5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -674,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="31.5">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -688,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -716,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="31.5">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -730,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="31.5">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -738,7 +738,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -835,19 +835,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -996,7 +996,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:7" ht="47.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45">
+    <row r="13" spans="1:7" ht="47.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1073,16 +1073,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1108,7 +1108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="31.5">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="47.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="31.5">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Updated sprint backlog and switched person numbers.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\2014-2015\Fall 2014\CS 2340 Objects and Design\SpaceTraders2340\admin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -141,8 +146,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -591,19 +596,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -619,14 +624,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
@@ -634,7 +639,7 @@
     <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -674,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5">
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -688,12 +693,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5">
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -701,13 +706,16 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="31.5">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -716,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -730,7 +738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -744,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -758,12 +766,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -772,12 +780,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>3</v>
@@ -786,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -800,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -814,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -835,19 +843,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -884,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -898,7 +906,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -912,7 +920,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -926,7 +934,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -940,7 +948,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -954,7 +962,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -968,7 +976,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -982,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -996,7 +1004,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="47.25">
+    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1010,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="31.5">
+    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1024,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="47.25">
+    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1046,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1052,7 +1060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1073,19 +1081,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
     <col min="3" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1122,7 +1130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="47.25">
+    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1150,7 +1158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1164,7 +1172,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Edited Sprint Backlog after JavaFX project was created.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\2014-2015\Fall 2014\CS 2340 Objects and Design\SpaceTraders2340\admin\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Tasks</t>
   </si>
@@ -133,6 +138,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -595,12 +603,12 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -623,15 +631,15 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -668,7 +676,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,7 +690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -696,7 +704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -710,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -724,7 +732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -738,7 +746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -752,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -766,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -780,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -794,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -808,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -833,15 +841,15 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -878,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -892,7 +900,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -906,7 +914,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -920,7 +928,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -934,7 +942,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -948,7 +956,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -962,21 +970,24 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -990,7 +1001,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1018,7 +1029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45">
+    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1032,7 +1043,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1046,7 +1057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1072,14 +1083,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1102,7 +1113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1116,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1141,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1144,7 +1155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1158,7 +1169,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1172,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Updated sprint backlog and added entries for use cases.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
   <si>
     <t>Tasks</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>UC1: Start Game</t>
+  </si>
+  <si>
+    <t>UC2: Create Character</t>
+  </si>
+  <si>
+    <t>UC5: Buy New Goods</t>
+  </si>
+  <si>
+    <t>UC9: Leave Project</t>
+  </si>
+  <si>
+    <t>UC6: Upgrade/Repair Ship</t>
   </si>
 </sst>
 </file>
@@ -838,10 +853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -891,32 +906,50 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>0.5</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>0.5</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -925,26 +958,26 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
@@ -953,49 +986,40 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
@@ -1004,81 +1028,104 @@
         <v>37</v>
       </c>
       <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
         <v>1.5</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13">
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="5">
-        <f>SUM(D2:D14)</f>
-        <v>14</v>
+      <c r="D16" s="5">
+        <f>SUM(D2:D15)</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished my use case, changed 'Start Game' to 'Load Game', and updated backlog.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -856,7 +856,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -955,10 +955,19 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set up New Game Window with fully functional increment/decrement actions. Updated sprint backlog.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Dropbox\2014-2015\Fall 2014\CS 2340 Objects and Design\SpaceTraders2340\admin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17475" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -603,12 +598,12 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -631,15 +626,15 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="2"/>
+    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="31.5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -676,7 +671,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="31.5">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -690,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -704,7 +699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -718,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="31.5">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -732,7 +727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="31.5">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -746,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -760,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -774,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -788,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -802,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -816,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -841,15 +836,15 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.125" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,12 +867,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -886,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -900,7 +895,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -914,7 +909,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -928,7 +923,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -942,7 +937,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -956,7 +951,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -970,7 +965,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -993,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1016,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="47.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1038,13 +1033,13 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="47.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1058,7 +1053,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1072,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1098,14 +1093,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="31.5">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1142,7 +1137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="47.25">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1156,7 +1151,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -1170,7 +1165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1184,7 +1179,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="31.5">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1198,7 +1193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
When play button is pressed, player object is created with designated name and skill points. When cancel button is pressed, New Game window closes. Updated sprint backlog.
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -141,8 +141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -591,16 +591,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -619,19 +619,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -832,16 +832,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1025,7 +1025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="31.5">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>1.5</v>
@@ -1088,16 +1088,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Updating Sprint Backlog after implementing game config to the New Game
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -141,13 +141,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -591,16 +592,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -619,19 +620,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="2"/>
+    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -657,7 +658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -671,7 +672,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -685,7 +686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -699,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -713,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -727,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -832,19 +833,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.125" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="47.25">
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1019,13 +1020,16 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.5">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1039,7 +1043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="47.25">
+    <row r="13" spans="1:7" ht="45">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1088,16 +1092,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1123,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="47.25">
+    <row r="3" spans="1:7" ht="45">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1179,7 +1183,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Uploaded new sprint backlog to include M5
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1540" yWindow="620" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
     <sheet name="Sprint 2 (M2)" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 5 (M5)" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Tasks</t>
   </si>
@@ -151,6 +152,36 @@
   </si>
   <si>
     <t>UC8: Refuel Ship</t>
+  </si>
+  <si>
+    <t>Link game screen to market screen</t>
+  </si>
+  <si>
+    <t>Create market screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naman </t>
+  </si>
+  <si>
+    <t>Create ship class to store all relevant data</t>
+  </si>
+  <si>
+    <t>Add money to player class (add limitation)</t>
+  </si>
+  <si>
+    <t>Make individual analysis diagrams</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>MarketController (calculating prices and resources)</t>
+  </si>
+  <si>
+    <t>MarketController(buying,selling,link controller to front-end)</t>
+  </si>
+  <si>
+    <t>Code review/javadoc</t>
   </si>
 </sst>
 </file>
@@ -214,8 +245,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,7 +284,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -261,6 +294,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -270,6 +304,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -850,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1264,4 +1299,174 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60">
+      <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
+        <f>SUM(D2:D7)</f>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sprint backlog to include M6
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="620" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="10520" yWindow="720" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sprint 3 (M3)" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
     <sheet name="Sprint 5 (M5)" sheetId="6" r:id="rId5"/>
+    <sheet name="Sprint 6 (M6)" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
   <si>
     <t>Tasks</t>
   </si>
@@ -182,6 +183,24 @@
   </si>
   <si>
     <t>Code review/javadoc</t>
+  </si>
+  <si>
+    <t>Package Diagram/ Trust boundaries</t>
+  </si>
+  <si>
+    <t>Algorithm for finding planets nearby by fuel and distance</t>
+  </si>
+  <si>
+    <t>Encounter with pirates and police</t>
+  </si>
+  <si>
+    <t>UI for encounter</t>
+  </si>
+  <si>
+    <t>UI for nearby planets</t>
+  </si>
+  <si>
+    <t>Code review/ Javadoc</t>
   </si>
 </sst>
 </file>
@@ -245,8 +264,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,7 +317,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -295,6 +328,13 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -305,6 +345,13 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1305,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1469,4 +1516,117 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sprint backlog tasks
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10520" yWindow="720" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -213,6 +213,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1523,7 +1524,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1614,7 +1615,7 @@
         <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>2</v>

</xml_diff>

<commit_message>
Updated sprint backlog with M7 tasks
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="13960" yWindow="0" windowWidth="13960" windowHeight="17560" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sprint 4 (M4)" sheetId="4" r:id="rId4"/>
     <sheet name="Sprint 5 (M5)" sheetId="6" r:id="rId5"/>
     <sheet name="Sprint 6 (M6)" sheetId="7" r:id="rId6"/>
+    <sheet name="Sprint 7 (M7)" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
   <si>
     <t>Tasks</t>
   </si>
@@ -201,6 +202,21 @@
   </si>
   <si>
     <t>Code review/ Javadoc</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Save/Load State (UI and controller and everything)</t>
+  </si>
+  <si>
+    <t>Naman/ Pranil</t>
+  </si>
+  <si>
+    <t>Code Critique and Java Doc</t>
+  </si>
+  <si>
+    <t>Random event generation and implementation and extra credit</t>
   </si>
 </sst>
 </file>
@@ -213,7 +229,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,8 +280,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,7 +335,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +353,7 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -353,6 +371,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1523,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1630,4 +1649,83 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="53.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sprint backlog to include M8
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="0" windowWidth="13960" windowHeight="17560" tabRatio="500" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="12860" yWindow="300" windowWidth="14400" windowHeight="16560" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Sprint 5 (M5)" sheetId="6" r:id="rId5"/>
     <sheet name="Sprint 6 (M6)" sheetId="7" r:id="rId6"/>
     <sheet name="Sprint 7 (M7)" sheetId="8" r:id="rId7"/>
+    <sheet name="Sprint 8 (M8)" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
   <si>
     <t>Tasks</t>
   </si>
@@ -217,6 +218,24 @@
   </si>
   <si>
     <t>Random event generation and implementation and extra credit</t>
+  </si>
+  <si>
+    <t>Individual sequence diagram</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Make a ship class with given attributes (similar to resource.java) and shipyard class</t>
+  </si>
+  <si>
+    <t>Sthephen</t>
+  </si>
+  <si>
+    <t>Make a shipyard view and a controller and implement controller with GUI</t>
+  </si>
+  <si>
+    <t>Bhavesh, Naman, Pranil</t>
   </si>
 </sst>
 </file>
@@ -280,8 +299,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,7 +360,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +379,9 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -372,6 +400,9 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1373,7 +1404,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1543,7 +1574,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1655,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1722,6 +1753,87 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="72.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Sprint Backlog for M9
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12860" yWindow="300" windowWidth="14400" windowHeight="16560" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="14400" yWindow="-20" windowWidth="14400" windowHeight="17460" tabRatio="500" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Sprint 6 (M6)" sheetId="7" r:id="rId6"/>
     <sheet name="Sprint 7 (M7)" sheetId="8" r:id="rId7"/>
     <sheet name="Sprint 8 (M8)" sheetId="9" r:id="rId8"/>
+    <sheet name="Spring 9 (M9)" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="75">
   <si>
     <t>Tasks</t>
   </si>
@@ -236,6 +237,21 @@
   </si>
   <si>
     <t>Bhavesh, Naman, Pranil</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Method Contracts (individual)</t>
+  </si>
+  <si>
+    <t>Ensure shipyard available at tech planets/Implement Option to Upgrade Ship</t>
+  </si>
+  <si>
+    <t>Enforce money/slot limits for upgrading ship. Enforce some gadgets only available on higher tech level planet</t>
+  </si>
+  <si>
+    <t>Apply design pattern to code</t>
   </si>
 </sst>
 </file>
@@ -299,8 +315,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -360,7 +380,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -382,6 +402,8 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -403,6 +425,8 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1766,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1840,4 +1864,90 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="90.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sprint backlog to current status
</commit_message>
<xml_diff>
--- a/admin/sprint_backlog.xlsx
+++ b/admin/sprint_backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="14400" windowHeight="16540" tabRatio="500" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="23420" windowHeight="16540" tabRatio="500" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 1 (M1)" sheetId="3" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="Sprint 8 (M8)" sheetId="9" r:id="rId8"/>
     <sheet name="Spring 9 (M9)" sheetId="10" r:id="rId9"/>
     <sheet name="Sprint 10 (M10)" sheetId="11" r:id="rId10"/>
+    <sheet name="Sprint 11 (M11)" sheetId="12" r:id="rId11"/>
+    <sheet name="Sprint 12 (M12)" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="82">
   <si>
     <t>Tasks</t>
   </si>
@@ -39,9 +41,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Hunter</t>
   </si>
   <si>
@@ -135,9 +134,6 @@
     <t>Cleanup, readover, code critique</t>
   </si>
   <si>
-    <t xml:space="preserve">Not Started </t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -225,24 +221,15 @@
     <t>Individual sequence diagram</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Make a ship class with given attributes (similar to resource.java) and shipyard class</t>
   </si>
   <si>
-    <t>Sthephen</t>
-  </si>
-  <si>
     <t>Make a shipyard view and a controller and implement controller with GUI</t>
   </si>
   <si>
     <t>Bhavesh, Naman, Pranil</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Method Contracts (individual)</t>
   </si>
   <si>
@@ -268,6 +255,27 @@
   </si>
   <si>
     <t>PMD</t>
+  </si>
+  <si>
+    <t>Invidual</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Usability Evaluation</t>
+  </si>
+  <si>
+    <t>Execute the plan</t>
+  </si>
+  <si>
+    <t>Usability Report</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Individual Design Review</t>
   </si>
 </sst>
 </file>
@@ -331,8 +339,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -398,7 +418,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -423,6 +443,12 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -447,6 +473,12 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,7 +829,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -812,10 +844,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -848,68 +880,337 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <f xml:space="preserve"> SUM(D2:D5)</f>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="33" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <f xml:space="preserve"> SUM(D2:D6)</f>
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -926,7 +1227,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -962,13 +1263,13 @@
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>0.5</v>
@@ -976,13 +1277,13 @@
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -990,13 +1291,13 @@
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -1004,13 +1305,13 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -1018,13 +1319,13 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -1032,13 +1333,13 @@
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -1046,13 +1347,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1060,13 +1361,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -1074,13 +1375,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1088,13 +1389,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1102,13 +1403,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1116,7 +1417,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1">
         <f>SUM(D2:D12)</f>
@@ -1139,7 +1440,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1172,13 +1473,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1186,13 +1487,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -1209,13 +1510,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>0.5</v>
@@ -1232,13 +1533,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1246,13 +1547,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1260,13 +1561,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1274,13 +1575,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1288,13 +1589,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1305,13 +1606,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1328,13 +1629,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>1.5</v>
@@ -1351,13 +1652,13 @@
     </row>
     <row r="12" spans="1:7" ht="45">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1368,13 +1669,13 @@
     </row>
     <row r="13" spans="1:7" ht="30">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1382,13 +1683,13 @@
     </row>
     <row r="14" spans="1:7" ht="45">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <v>1.5</v>
@@ -1396,10 +1697,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>35</v>
@@ -1410,7 +1711,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="5">
         <f>SUM(D2:D15)</f>
@@ -1432,7 +1733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1466,13 +1769,13 @@
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -1480,13 +1783,13 @@
     </row>
     <row r="3" spans="1:7" ht="45">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>1.5</v>
@@ -1494,13 +1797,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -1508,13 +1811,13 @@
     </row>
     <row r="5" spans="1:7" ht="30">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>1.5</v>
@@ -1522,10 +1825,10 @@
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>35</v>
@@ -1536,7 +1839,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1">
         <f>SUM(D2:D6)</f>
@@ -1559,7 +1862,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1594,13 +1897,13 @@
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -1608,13 +1911,13 @@
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>1.5</v>
@@ -1622,13 +1925,13 @@
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -1636,13 +1939,13 @@
     </row>
     <row r="5" spans="1:7" ht="45">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1650,13 +1953,13 @@
     </row>
     <row r="6" spans="1:7" ht="60">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D6" s="2">
         <v>1.5</v>
@@ -1664,12 +1967,12 @@
     </row>
     <row r="7" spans="1:7" ht="45">
       <c r="A7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="2">
@@ -1678,13 +1981,13 @@
     </row>
     <row r="8" spans="1:7" ht="30">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="2">
         <v>1.5</v>
@@ -1692,13 +1995,13 @@
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="2">
         <v>1.5</v>
@@ -1706,7 +2009,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1">
         <f>SUM(D2:D7)</f>
@@ -1729,7 +2032,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1762,10 +2065,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1773,10 +2079,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1784,10 +2093,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1795,10 +2107,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1806,10 +2121,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1817,10 +2135,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1839,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:G5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1876,34 +2197,67 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1919,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1956,34 +2310,67 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1999,10 +2386,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2035,42 +2422,81 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>